<commit_message>
added report checklist file 14_07_2025
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#SYNCLINEXX/Sync-Line_Studio_Srls/NetClinic/v.1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#SYNCLINEXX/Sync-Line_Studio_Srls/NetClinic/v.1.0/report-checklist.xlsx
@@ -7,14 +7,17 @@
     <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
   </bookViews>
   <sheets>
-    <sheet name="TestCases" sheetId="1" r:id="rId1"/>
+    <sheet name="Istruzioni Compilazione" sheetId="2" r:id="rId1"/>
+    <sheet name="Prerequisiti" sheetId="3" r:id="rId2"/>
+    <sheet name="TestCases" sheetId="1" r:id="rId3"/>
+    <sheet name="Summary" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="70">
   <si>
     <t>NOME FORNITORE:</t>
   </si>
@@ -92,9 +95,6 @@
 Publish - "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents"</t>
   </si>
   <si>
-    <t>ok</t>
-  </si>
-  <si>
     <t>2025-07-09T08:00:42Z</t>
   </si>
   <si>
@@ -156,6 +156,146 @@
   </si>
   <si>
     <t>subject_application_version: v.1.0</t>
+  </si>
+  <si>
+    <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Necessario compilare sempre le righe 2,3,4,5 con rispettivamente:
+Nome fornitore dell'applicativo
+nome applicazione: subject_application_id
+Nome fornitore: subject_application_vendor
+versione applicazione: subject_application_version
+</t>
+  </si>
+  <si>
+    <t>2) Per tutti i casi di test coerenti con la/e tipologia/e di documento utilizzata/e dal software è necessario compilare SEMPRE la colonna APPLICABILITA' con SI o NO</t>
+  </si>
+  <si>
+    <t>4) Se il test è applicabile la colonna APPLICABILITA' deve essere compilata con SI e dovranno essere valorizzate:
+    DATA ESECUZIONE, 
+    TIMESTAMP, 
+    TRACEID,
+    WORKFLOWINSTANCEID (ove ritornato in response, qualora non ritornato il WORKFLOWINSTANCEID puo' essere lasciato blank), 
+    ERRORE BLOCCANTE (SI/NO) da compilare solo per i casi KO (ovvero con colonna CASO OK / KO= KO) e per i casi di test di TIMEOUT,
+    ERRORE VISIBILE A UTENTE (SI/NO) da compilare solo per i casi KO (ovvero con colonna CASO OK / KO= KO) e per i casi di test di TIMEOUT,
+    MESSAGGIO DI ERRORE da compilare con il messaggio di errore visualizzato dall’applicativo, solo per i casi KO (ovvero con colonna CASO OK / KO= KO) e per i casi di test di TIMEOUT visibili all'utente (colonna ERRORE VISIBILE A UTENTE (SI/NO)=SI)
+    GESTITO IN BACKOFFICE (SI/NO) da compilare solo per i casi KO (ovvero con colonna CASO OK / KO= KO) e per i casi di test di TIMEOUT,
+    PRESENTE CODA DI RETRY AUTOMATICA PER L'INVIO DEL DOCUMENTO A FSE A SEGUITO DELLA RISOLUZIONE DELL'ERRORE (SI/NO) da compilare solo per i casi KO (ovvero con colonna CASO OK / KO= KO) e per i casi di test di TIMEOUT,
+   INVIO MANUALE DEL DOCUMENTO AL FSE A SEGUITO DELLA RISOLUZIONE DELL'ERRORE (SI/NO) da compilare solo per i casi KO  (ovvero con colonna CASO OK / KO= KO) e per i casi di test di TIMEOUT,
+    GESTIONE ERRORE da compilare con la procedura che viene adottata per la gestione dell'errore, solo per i casi KO (ovvero con CASO OK / KO= KO) e per i casi di test di TIMEOUT,  specificando le modalità di invio del documento clinico al FSE a seguito della correzione dell'errore e chiarendo se è possibile per l'utente (medico) proseguire con il processo e produrre il documento. Esclusivamente per i casi di test di TIMEOUT, qualora non fosse prevista una coda di retry e la gestione dell'errore non fossa gestita da un operatore di backoffice, indicare le modalità attraverso cui è reso esplicito all’utente (medico) di effettuare nuovi tentativi di invio verso il FSE fino al ripristino del servizio di validazione.</t>
+  </si>
+  <si>
+    <t>COME VALORIZZARE I DATAJSON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) E' necessario seguire le istruzioni fornite al path github.com/ministero-salute/it-fse-accreditamento, sezione "Struttura dei risultati (data.json)" con l'accortezza di utilizzare come "id" in "results", gli stessi identificativi di test effettuati. Questi sono recuperabili dalla colonna ID del tab TestCases. </t>
+  </si>
+  <si>
+    <t>2) E' necessario compilare i datajson per tutti i casi OK/KO applicabili.</t>
+  </si>
+  <si>
+    <t>PREREQUISITI</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Obiettivo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: In questo foglio si riportano i pre requisiti/assunzioni necessari all'accreditamento del software dei </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>client</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> che ne hanno fatto richiesta, e utili alla compilazione della presente Checklist.</t>
+    </r>
+  </si>
+  <si>
+    <t>Per gli step precedenti alla Checklist e relativi allo sviluppo per l'integrazione con il Gateway, è necessario fare riferimento al portale https://developers.italia.it/it/fse/#resourcecontent-2</t>
+  </si>
+  <si>
+    <t>Il fornitore prima di procedere con la compilazione di questo xls, deve aver richiesto a Sogei le credenziali (fse_support@sogei.it fino a quando non sarà disponibile il sistema di provisioning) associate al fornitore per accedere ai servizi esposti dalla piattaforma Gateway di test in ambiente di pre produzione.</t>
+  </si>
+  <si>
+    <t>il fornitore, prima di procedere con la Checklist, risulta autenticato secondo quanto definito nelle specifiche "https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway"</t>
+  </si>
+  <si>
+    <t>Il fornitore comunica al DTD e Sogei:
+a. nome del fornitore
+b. identificativi del software oggetto dell’accreditamento (metadati che dovranno essere inseriti nel token JWT): subject_application_id, subject_application_vendor, subject_application_version
+c. inizio della sessione di accreditamento
+d. tipi di documento e servizi che sono oggetto dell’accreditamento</t>
+  </si>
+  <si>
+    <r>
+      <t>I file CDA2 necessari all'esecuzione dei test di accreditamento devono essere costruiti secondo le specifiche nazionali https://www.hl7.it/realm-italiano/ e coerentemente ai casi di test descritti.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>TIPO DOCUMENTO</t>
+  </si>
+  <si>
+    <t>ID TEST CASE OK</t>
+  </si>
+  <si>
+    <t>ID TEST CASE KO</t>
+  </si>
+  <si>
+    <t>Versione:</t>
+  </si>
+  <si>
+    <t>8.2.6</t>
+  </si>
+  <si>
+    <t>Validazione</t>
+  </si>
+  <si>
+    <t>4,5,6,7,8</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LAB_CT4</t>
+  </si>
+  <si>
+    <t>3) Nel caso in cui tra le tipologie documentali oggetto di accreditamento per l'applicativo figurino LAB i relativi casi di test con id 452,450 che recepiscono quanto previsto dal Decreto  07 settembre 2023, devono essere obbligatoriamente eseguiti e compilati (la colonna APPLICABILITA' deve essere valorizzata con SI)</t>
+  </si>
+  <si>
+    <t>5) Se il test NON è applicabile la colonna APPLICABILITA' riporterà NO e dovrà essere compilata esclusivamente la colonna RAZIONALE DI APPLICABILITA' con le motivazioni per cui il test non è applicabile. Il campo è valorizzabile tramite selezione da menù a tendina (campo/sezione non gestito/a in modo strutturato dall’applicativo;c ampo obbligatorio; campo valorizzato di default; campo valorizzato in automatico tramite dati recuperati da servizi esterni; campo valorizzabile tramite selezione da un set di valori ammessi; l’applicativo effettua controlli preventivi sul dato inserito; altro (specificare)). Nel caso in cui si selezioni l'opzione "Altro (specificare)" è necessario compilare la colonna RAZIONALE DI "APPLICABILITA' - ALTRO" con le motivazioni per le quali il test non è applicabile.</t>
   </si>
 </sst>
 </file>
@@ -165,7 +305,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,19 +353,96 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF1F2328"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -238,28 +455,25 @@
         <bgColor rgb="FF666699"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4472C4"/>
+        <bgColor rgb="FF4472C4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="12">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -329,63 +543,287 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="12" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="12" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="14" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="14" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="16"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="16" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="7" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="18" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="19">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 10" xfId="14"/>
+    <cellStyle name="Normal 11" xfId="16"/>
     <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2 2" xfId="5"/>
+    <cellStyle name="Normal 2 3" xfId="7"/>
+    <cellStyle name="Normal 2 4" xfId="9"/>
+    <cellStyle name="Normal 2 5" xfId="11"/>
+    <cellStyle name="Normal 2 6" xfId="13"/>
+    <cellStyle name="Normal 2 7" xfId="15"/>
+    <cellStyle name="Normal 2 8" xfId="17"/>
+    <cellStyle name="Normal 2 9" xfId="18"/>
     <cellStyle name="Normal 3" xfId="2"/>
     <cellStyle name="Normal 4" xfId="3"/>
+    <cellStyle name="Normal 5" xfId="4"/>
+    <cellStyle name="Normal 6" xfId="6"/>
+    <cellStyle name="Normal 7" xfId="8"/>
+    <cellStyle name="Normal 8" xfId="10"/>
+    <cellStyle name="Normal 9" xfId="12"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E2F3"/>
+          <bgColor rgb="FFD9E2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E2F3"/>
+          <bgColor rgb="FFD9E2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E2F3"/>
+          <bgColor rgb="FFD9E2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E2F3"/>
+          <bgColor rgb="FFD9E2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="2">
+    <tableStyle name="Sheet1-style" pivot="0" count="3">
+      <tableStyleElement type="headerRow" dxfId="5"/>
+      <tableStyleElement type="firstRowStripe" dxfId="4"/>
+      <tableStyleElement type="secondRowStripe" dxfId="3"/>
+    </tableStyle>
+    <tableStyle name="Sheet1-style 2" pivot="0" count="3">
+      <tableStyleElement type="headerRow" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="secondRowStripe" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
 </styleSheet>
 </file>
 
@@ -674,23 +1112,142 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="108.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="90">
+      <c r="A2" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="30">
+      <c r="A3" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="45">
+      <c r="A4" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="285">
+      <c r="A5" s="18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="105">
+      <c r="A6" s="35" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="45">
+      <c r="A8" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="178" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="19.5" thickBot="1">
+      <c r="A1" s="21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75" thickTop="1">
+      <c r="A2" s="22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" thickBot="1">
+      <c r="A3" s="22"/>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="30">
+      <c r="A5" s="24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="30">
+      <c r="A6" s="24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="75">
+      <c r="A7" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:T12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="76.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" style="10" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" style="9" customWidth="1"/>
     <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.5703125" style="8" customWidth="1"/>
-    <col min="9" max="9" width="32.85546875" style="8" customWidth="1"/>
+    <col min="8" max="8" width="35.5703125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="32.85546875" style="7" customWidth="1"/>
     <col min="10" max="10" width="16.5703125" customWidth="1"/>
     <col min="11" max="11" width="17.7109375" customWidth="1"/>
     <col min="12" max="12" width="19.140625" customWidth="1"/>
@@ -703,41 +1260,41 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:20">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:20">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="15"/>
+      <c r="B3" s="13"/>
       <c r="C3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:20">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:20">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:20" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:20" s="6" customFormat="1" ht="26.25" thickBot="1">
+    <row r="7" spans="1:20" s="6" customFormat="1" ht="25.5">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -753,16 +1310,16 @@
       <c r="E7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="10" t="s">
         <v>8</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="8" t="s">
         <v>11</v>
       </c>
       <c r="J7" s="4" t="s">
@@ -799,239 +1356,239 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="76.5" thickBot="1">
+    <row r="8" spans="1:20" ht="75">
       <c r="A8">
         <v>4</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>44</v>
+      <c r="C8" s="33" t="s">
+        <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="9">
         <v>45847</v>
       </c>
       <c r="G8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="J8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L8" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="L8" s="8" t="s">
+      <c r="M8" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="O8" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q8" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="M8" s="8" t="s">
+      <c r="T8" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="O8" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q8" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="T8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" ht="76.5" thickBot="1">
+    </row>
+    <row r="9" spans="1:20" ht="75">
       <c r="A9">
         <v>5</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>44</v>
+      <c r="C9" s="33" t="s">
+        <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="9">
         <v>45847</v>
       </c>
       <c r="G9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="J9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L9" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="L9" s="8" t="s">
+      <c r="M9" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q9" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="M9" s="8" t="s">
+      <c r="T9" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="O9" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q9" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="T9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" ht="76.5" thickBot="1">
+    </row>
+    <row r="10" spans="1:20" ht="75">
       <c r="A10">
         <v>6</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>44</v>
+      <c r="C10" s="33" t="s">
+        <v>43</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="9">
         <v>45847</v>
       </c>
       <c r="G10" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="J10" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L10" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="L10" s="8" t="s">
+      <c r="M10" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q10" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="M10" s="8" t="s">
+      <c r="T10" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="O10" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q10" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="T10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" ht="76.5" thickBot="1">
+    </row>
+    <row r="11" spans="1:20" ht="75">
       <c r="A11">
         <v>7</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>44</v>
+      <c r="C11" s="33" t="s">
+        <v>43</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="9">
         <v>45847</v>
       </c>
       <c r="G11" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="J11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L11" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="L11" s="8" t="s">
+      <c r="M11" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q11" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="M11" s="8" t="s">
+      <c r="T11" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="O11" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q11" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="T11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" ht="75.75">
+    </row>
+    <row r="12" spans="1:20" ht="75">
       <c r="A12">
         <v>8</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>44</v>
+      <c r="C12" s="33" t="s">
+        <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="9">
         <v>45847</v>
       </c>
       <c r="G12" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="I12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="L12" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="L12" s="8" t="s">
+      <c r="M12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="O12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q12" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="M12" s="8" t="s">
+      <c r="T12" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="O12" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q12" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="T12" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1043,4 +1600,64 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A1" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="25"/>
+      <c r="F1" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="30"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>